<commit_message>
feat(fe): basic requirements meet, still missing fancy stuff
</commit_message>
<xml_diff>
--- a/samples/senior15nope.xlsx
+++ b/samples/senior15nope.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">puturrudefua</t>
+    <t xml:space="preserve">senior</t>
   </si>
 </sst>
 </file>
@@ -249,8 +249,7 @@
       <c r="B1" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="C1" s="2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>